<commit_message>
[feature] Notebook components process, line infos and simplify logs
</commit_message>
<xml_diff>
--- a/Planilha de Input.xlsx
+++ b/Planilha de Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OneDriveFalse\1 - KevDev\2 - Estudos\Testes de codigo\GLPI scripts\Input de informações e criação de coisas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B19172-B91E-4C62-8011-1411EEB79972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560162F8-D0B0-4470-AFB1-ED62D33C02FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="1968" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="96">
   <si>
     <t>Nome do User</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t>Reparo</t>
+  </si>
+  <si>
+    <t>TIPO</t>
   </si>
 </sst>
 </file>
@@ -658,9 +661,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM12"/>
+  <dimension ref="A1:AN12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AE2" sqref="AE2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -689,16 +694,17 @@
     <col min="28" max="28" width="20" customWidth="1"/>
     <col min="29" max="29" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="26.28515625" customWidth="1"/>
+    <col min="32" max="32" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -789,35 +795,38 @@
       <c r="AD1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AE1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -861,7 +870,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -887,7 +896,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -922,7 +931,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -933,7 +942,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -953,7 +962,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -979,7 +988,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1005,7 +1014,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1031,7 +1040,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1054,7 +1063,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -1077,7 +1086,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>49</v>
       </c>

</xml_diff>